<commit_message>
Adicionando material do vídeo 1 de OpenPyXL
</commit_message>
<xml_diff>
--- a/OpenPyXL/001_Funções_Básicas/planilha.xlsx
+++ b/OpenPyXL/001_Funções_Básicas/planilha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python_Tutoriais\OpenPyXL\001_Funções_Básicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69361C5-6DCD-410F-BF7E-470D5A8D45F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C62B60-255F-4D1D-91AE-7D4BC1FD5910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="1845" windowWidth="21667" windowHeight="11333" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5573" yWindow="2183" windowWidth="21667" windowHeight="11332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -95,10 +95,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
@@ -385,81 +384,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="1"/>
-    <col min="2" max="2" width="13.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>2500</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>5500</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>120</v>
       </c>
     </row>

</xml_diff>